<commit_message>
spreadsheets: Add cover sheet "Introduction" with spreadsheet version
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/fund.xlsx
+++ b/indigo/spreadsheetform_guides/fund.xlsx
@@ -8,8 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="General Overview" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Organisations" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="General Overview" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Organisations" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,12 +22,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">INDIGO Fund ID</t>
+  </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:id</t>
   </si>
   <si>
     <t xml:space="preserve">(Can not be changed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Do not change the layout of this spreadsheet or add extra details. This will not be picked up, and it may result in data being lost.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEET VERSION</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -301,10 +311,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,53 +382,44 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>1</v>
-      </c>
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -376,7 +432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -395,12 +451,12 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>